<commit_message>
add notes on marr vars
</commit_message>
<xml_diff>
--- a/marriage-vars-map.xlsx
+++ b/marriage-vars-map.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sacfiles1\home\m\maxbnorton\Documents\ECON 200C\500_data\500_data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27729"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12440"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>willMarryN</t>
   </si>
@@ -105,13 +103,19 @@
   </si>
   <si>
     <t>1. currently = 0 in 1965 no matter what. But shouldn't it = 1 if married pre-65?</t>
+  </si>
+  <si>
+    <t>increases standard error of est coefficients of regional marriage vars. Effect size is derivable regardless. So I think this is unnecessary.</t>
+  </si>
+  <si>
+    <t>separate marriage effect from marriage to region effect</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +129,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -148,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -160,10 +170,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -225,7 +244,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -260,7 +279,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,7 +456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -448,16 +467,16 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="G11" sqref="G11:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="2"/>
-    <col min="2" max="16384" width="19.85546875" style="1"/>
+    <col min="1" max="1" width="19.83203125" style="2"/>
+    <col min="2" max="16384" width="19.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="3" customFormat="1">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -484,7 +503,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -500,7 +519,7 @@
       <c r="E2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -509,120 +528,120 @@
       <c r="H2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F4" s="5"/>
-      <c r="I4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F5" s="5"/>
-      <c r="I5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" s="5"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
+      <c r="F3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="F4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="F5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="F6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="F7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="F8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="F9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="4"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -638,36 +657,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" ht="42">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" ht="84">
       <c r="A25" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="B25" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="I2:I9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="H11:H13"/>
     <mergeCell ref="C15:C18"/>
     <mergeCell ref="H15:H18"/>
     <mergeCell ref="D11:D13"/>
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="D15:D18"/>
     <mergeCell ref="E15:E18"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="I2:I9"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="H11:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>